<commit_message>
feat: Implement smoke missile optimization system
Co-authored-by: 3349523701 <3349523701@qq.com>
</commit_message>
<xml_diff>
--- a/结果3.xlsx
+++ b/结果3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>飞行速度</t>
+          <t>飞行速度(m/s)</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -481,7 +481,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>飞行时间</t>
+          <t>飞行时间(s)</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -491,7 +491,7 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>投放时间</t>
+          <t>投放时间(s)</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
@@ -526,12 +526,12 @@
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>爆炸时间</t>
+          <t>爆炸时间(s)</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>遮蔽时间</t>
+          <t>遮蔽时间(s)</t>
         </is>
       </c>
     </row>
@@ -547,58 +547,58 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-0.99476</v>
+        <v>-0.993929</v>
       </c>
       <c r="D2" t="n">
-        <v>0.012181</v>
+        <v>0.019682</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.101506</v>
+        <v>-0.10825</v>
       </c>
       <c r="F2" t="n">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="G2" t="n">
-        <v>8000</v>
+        <v>15555.555556</v>
       </c>
       <c r="H2" t="n">
-        <v>120</v>
+        <v>44.444444</v>
       </c>
       <c r="I2" t="n">
-        <v>800</v>
+        <v>1555.555556</v>
       </c>
       <c r="J2" t="n">
-        <v>82.09682599999999</v>
+        <v>32.259342</v>
       </c>
       <c r="K2" t="n">
         <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>65.67746099999999</v>
+        <v>25.807474</v>
       </c>
       <c r="M2" t="n">
-        <v>9960</v>
+        <v>16004.444444</v>
       </c>
       <c r="N2" t="n">
-        <v>96</v>
+        <v>35.555556</v>
       </c>
       <c r="O2" t="n">
-        <v>1000</v>
+        <v>1604.444444</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>15555.555556</v>
       </c>
       <c r="Q2" t="n">
-        <v>200</v>
+        <v>44.444444</v>
       </c>
       <c r="R2" t="n">
         <v>80</v>
       </c>
       <c r="S2" t="n">
-        <v>67.67746099999999</v>
+        <v>17.638342</v>
       </c>
       <c r="T2" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -613,58 +613,58 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-0.99476</v>
+        <v>-0.993929</v>
       </c>
       <c r="D3" t="n">
-        <v>0.012181</v>
+        <v>0.019682</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.101506</v>
+        <v>-0.10825</v>
       </c>
       <c r="F3" t="n">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="G3" t="n">
-        <v>8000</v>
+        <v>15555.555556</v>
       </c>
       <c r="H3" t="n">
-        <v>120</v>
+        <v>44.444444</v>
       </c>
       <c r="I3" t="n">
-        <v>800</v>
+        <v>1555.555556</v>
       </c>
       <c r="J3" t="n">
-        <v>82.09682599999999</v>
+        <v>32.259342</v>
       </c>
       <c r="K3" t="n">
         <v>2</v>
       </c>
       <c r="L3" t="n">
-        <v>67.17746099999999</v>
+        <v>26.807474</v>
       </c>
       <c r="M3" t="n">
-        <v>9780.943139000001</v>
+        <v>15934.869422</v>
       </c>
       <c r="N3" t="n">
-        <v>98.192533</v>
+        <v>36.933279</v>
       </c>
       <c r="O3" t="n">
-        <v>981.728892</v>
+        <v>1596.866967</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>15555.555556</v>
       </c>
       <c r="Q3" t="n">
-        <v>200</v>
+        <v>44.444444</v>
       </c>
       <c r="R3" t="n">
         <v>80</v>
       </c>
       <c r="S3" t="n">
-        <v>69.17746099999999</v>
+        <v>17.59445</v>
       </c>
       <c r="T3" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -679,190 +679,190 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.99476</v>
+        <v>-0.993929</v>
       </c>
       <c r="D4" t="n">
-        <v>0.012181</v>
+        <v>0.019682</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.101506</v>
+        <v>-0.10825</v>
       </c>
       <c r="F4" t="n">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="G4" t="n">
-        <v>8000</v>
+        <v>15555.555556</v>
       </c>
       <c r="H4" t="n">
-        <v>120</v>
+        <v>44.444444</v>
       </c>
       <c r="I4" t="n">
-        <v>800</v>
+        <v>1555.555556</v>
       </c>
       <c r="J4" t="n">
-        <v>82.09682599999999</v>
+        <v>32.259342</v>
       </c>
       <c r="K4" t="n">
         <v>3</v>
       </c>
       <c r="L4" t="n">
-        <v>68.67746099999999</v>
+        <v>27.807474</v>
       </c>
       <c r="M4" t="n">
-        <v>9601.886278</v>
+        <v>15865.2944</v>
       </c>
       <c r="N4" t="n">
-        <v>100.385066</v>
+        <v>38.311002</v>
       </c>
       <c r="O4" t="n">
-        <v>963.4577839999999</v>
+        <v>1589.289489</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>15555.555556</v>
       </c>
       <c r="Q4" t="n">
-        <v>200</v>
+        <v>44.444444</v>
       </c>
       <c r="R4" t="n">
         <v>80</v>
       </c>
       <c r="S4" t="n">
-        <v>70.67746099999999</v>
+        <v>17.550449</v>
       </c>
       <c r="T4" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>M2</t>
+          <t>M1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>FY1</t>
+          <t>FY5</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.994986</v>
+        <v>-0.943454</v>
       </c>
       <c r="D5" t="n">
-        <v>0.035117</v>
+        <v>0.317795</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.09364599999999999</v>
+        <v>-0.094345</v>
       </c>
       <c r="F5" t="n">
-        <v>120</v>
+        <v>125.236448</v>
       </c>
       <c r="G5" t="n">
-        <v>7600</v>
+        <v>6666.666667</v>
       </c>
       <c r="H5" t="n">
-        <v>360</v>
+        <v>133.333333</v>
       </c>
       <c r="I5" t="n">
-        <v>840</v>
+        <v>666.666667</v>
       </c>
       <c r="J5" t="n">
-        <v>85.42833299999999</v>
+        <v>53.60199</v>
       </c>
       <c r="K5" t="n">
         <v>1</v>
       </c>
       <c r="L5" t="n">
-        <v>68.34266599999999</v>
+        <v>42.881592</v>
       </c>
       <c r="M5" t="n">
-        <v>9640</v>
+        <v>7933.333333</v>
       </c>
       <c r="N5" t="n">
-        <v>288</v>
+        <v>-293.333333</v>
       </c>
       <c r="O5" t="n">
-        <v>1032</v>
+        <v>793.333333</v>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>6666.666667</v>
       </c>
       <c r="Q5" t="n">
-        <v>200</v>
+        <v>133.333333</v>
       </c>
       <c r="R5" t="n">
         <v>80</v>
       </c>
       <c r="S5" t="n">
-        <v>70.34266599999999</v>
+        <v>12.06558</v>
       </c>
       <c r="T5" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>M2</t>
+          <t>M1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>FY1</t>
+          <t>FY5</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-0.994986</v>
+        <v>-0.943454</v>
       </c>
       <c r="D6" t="n">
-        <v>0.035117</v>
+        <v>0.317795</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.09364599999999999</v>
+        <v>-0.094345</v>
       </c>
       <c r="F6" t="n">
-        <v>120</v>
+        <v>125.236448</v>
       </c>
       <c r="G6" t="n">
-        <v>7600</v>
+        <v>6666.666667</v>
       </c>
       <c r="H6" t="n">
-        <v>360</v>
+        <v>133.333333</v>
       </c>
       <c r="I6" t="n">
-        <v>840</v>
+        <v>666.666667</v>
       </c>
       <c r="J6" t="n">
-        <v>85.42833299999999</v>
+        <v>53.60199</v>
       </c>
       <c r="K6" t="n">
         <v>2</v>
       </c>
       <c r="L6" t="n">
-        <v>69.84266599999999</v>
+        <v>43.881592</v>
       </c>
       <c r="M6" t="n">
-        <v>9460.902509</v>
+        <v>7815.178516</v>
       </c>
       <c r="N6" t="n">
-        <v>294.321088</v>
+        <v>-253.533816</v>
       </c>
       <c r="O6" t="n">
-        <v>1015.143766</v>
+        <v>781.5178519999999</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>6666.666667</v>
       </c>
       <c r="Q6" t="n">
-        <v>200</v>
+        <v>133.333333</v>
       </c>
       <c r="R6" t="n">
         <v>80</v>
       </c>
       <c r="S6" t="n">
-        <v>71.84266599999999</v>
+        <v>11.965238</v>
       </c>
       <c r="T6" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -877,64 +877,64 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.994986</v>
+        <v>-0.995014</v>
       </c>
       <c r="D7" t="n">
-        <v>0.035117</v>
+        <v>0.028925</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.09364599999999999</v>
+        <v>-0.095452</v>
       </c>
       <c r="F7" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="G7" t="n">
-        <v>7600</v>
+        <v>6333.333333</v>
       </c>
       <c r="H7" t="n">
-        <v>360</v>
+        <v>333.333333</v>
       </c>
       <c r="I7" t="n">
-        <v>840</v>
+        <v>700</v>
       </c>
       <c r="J7" t="n">
-        <v>85.42833299999999</v>
+        <v>82.315209</v>
       </c>
       <c r="K7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L7" t="n">
-        <v>71.34266599999999</v>
+        <v>65.85216699999999</v>
       </c>
       <c r="M7" t="n">
-        <v>9281.805017999999</v>
+        <v>8626.666667</v>
       </c>
       <c r="N7" t="n">
-        <v>300.642176</v>
+        <v>266.666667</v>
       </c>
       <c r="O7" t="n">
-        <v>998.2875309999999</v>
+        <v>920</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>6333.333333</v>
       </c>
       <c r="Q7" t="n">
-        <v>200</v>
+        <v>333.333333</v>
       </c>
       <c r="R7" t="n">
         <v>80</v>
       </c>
       <c r="S7" t="n">
-        <v>73.34266599999999</v>
+        <v>13.093073</v>
       </c>
       <c r="T7" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>M3</t>
+          <t>M2</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -943,191 +943,777 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.995158</v>
+        <v>-0.995014</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.011266</v>
+        <v>0.028925</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.097638</v>
+        <v>-0.095452</v>
       </c>
       <c r="F8" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="G8" t="n">
-        <v>7200</v>
+        <v>6333.333333</v>
       </c>
       <c r="H8" t="n">
-        <v>-120</v>
+        <v>333.333333</v>
       </c>
       <c r="I8" t="n">
-        <v>760</v>
+        <v>700</v>
       </c>
       <c r="J8" t="n">
-        <v>88.763105</v>
+        <v>82.315209</v>
       </c>
       <c r="K8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L8" t="n">
-        <v>71.01048400000001</v>
+        <v>66.85216699999999</v>
       </c>
       <c r="M8" t="n">
-        <v>9320</v>
+        <v>8487.364747</v>
       </c>
       <c r="N8" t="n">
-        <v>-96</v>
+        <v>270.716141</v>
       </c>
       <c r="O8" t="n">
-        <v>968</v>
+        <v>906.636734</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>6333.333333</v>
       </c>
       <c r="Q8" t="n">
-        <v>200</v>
+        <v>333.333333</v>
       </c>
       <c r="R8" t="n">
         <v>80</v>
       </c>
       <c r="S8" t="n">
-        <v>73.01048400000001</v>
+        <v>12.988509</v>
       </c>
       <c r="T8" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>M3</t>
+          <t>M2</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>FY1</t>
+          <t>FY5</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.995158</v>
+        <v>-0.709796</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.011266</v>
+        <v>0.7033430000000001</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.097638</v>
+        <v>-0.038716</v>
       </c>
       <c r="F9" t="n">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="G9" t="n">
-        <v>7200</v>
+        <v>10555.555556</v>
       </c>
       <c r="H9" t="n">
-        <v>-120</v>
+        <v>422.222222</v>
       </c>
       <c r="I9" t="n">
-        <v>760</v>
+        <v>1166.666667</v>
       </c>
       <c r="J9" t="n">
-        <v>88.763105</v>
+        <v>49.198156</v>
       </c>
       <c r="K9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L9" t="n">
-        <v>72.51048400000001</v>
+        <v>39.358525</v>
       </c>
       <c r="M9" t="n">
-        <v>9140.871521999999</v>
+        <v>11044.444444</v>
       </c>
       <c r="N9" t="n">
-        <v>-98.02786999999999</v>
+        <v>-62.222222</v>
       </c>
       <c r="O9" t="n">
-        <v>950.42513</v>
+        <v>1193.333333</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>10555.555556</v>
       </c>
       <c r="Q9" t="n">
-        <v>200</v>
+        <v>422.222222</v>
       </c>
       <c r="R9" t="n">
         <v>80</v>
       </c>
       <c r="S9" t="n">
-        <v>74.51048400000001</v>
+        <v>15.073516</v>
       </c>
       <c r="T9" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>M3</t>
+          <t>M2</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>FY1</t>
+          <t>FY5</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.995158</v>
+        <v>-0.709796</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.011266</v>
+        <v>0.7033430000000001</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.097638</v>
+        <v>-0.038716</v>
       </c>
       <c r="F10" t="n">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="G10" t="n">
-        <v>7200</v>
+        <v>10555.555556</v>
       </c>
       <c r="H10" t="n">
-        <v>-120</v>
+        <v>422.222222</v>
       </c>
       <c r="I10" t="n">
-        <v>760</v>
+        <v>1166.666667</v>
       </c>
       <c r="J10" t="n">
-        <v>88.763105</v>
+        <v>49.198156</v>
       </c>
       <c r="K10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L10" t="n">
-        <v>74.01048400000001</v>
+        <v>40.358525</v>
       </c>
       <c r="M10" t="n">
-        <v>8961.743044000001</v>
+        <v>10994.758752</v>
       </c>
       <c r="N10" t="n">
-        <v>-100.055739</v>
+        <v>-12.988218</v>
       </c>
       <c r="O10" t="n">
-        <v>932.850261</v>
+        <v>1190.623205</v>
       </c>
       <c r="P10" t="n">
-        <v>0</v>
+        <v>10555.555556</v>
       </c>
       <c r="Q10" t="n">
-        <v>200</v>
+        <v>422.222222</v>
       </c>
       <c r="R10" t="n">
         <v>80</v>
       </c>
       <c r="S10" t="n">
-        <v>76.01048400000001</v>
+        <v>15.055158</v>
       </c>
       <c r="T10" t="n">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>M2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>FY5</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>-0.709796</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.7033430000000001</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-0.038716</v>
+      </c>
+      <c r="F11" t="n">
+        <v>70</v>
+      </c>
+      <c r="G11" t="n">
+        <v>10555.555556</v>
+      </c>
+      <c r="H11" t="n">
+        <v>422.222222</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1166.666667</v>
+      </c>
+      <c r="J11" t="n">
+        <v>49.198156</v>
+      </c>
+      <c r="K11" t="n">
+        <v>3</v>
+      </c>
+      <c r="L11" t="n">
+        <v>41.358525</v>
+      </c>
+      <c r="M11" t="n">
+        <v>10945.07306</v>
+      </c>
+      <c r="N11" t="n">
+        <v>36.245786</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1187.913076</v>
+      </c>
+      <c r="P11" t="n">
+        <v>10555.555556</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>422.222222</v>
+      </c>
+      <c r="R11" t="n">
+        <v>80</v>
+      </c>
+      <c r="S11" t="n">
+        <v>15.036779</v>
+      </c>
+      <c r="T11" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>M3</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>FY1</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>-0.994957</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.006997</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-0.100055</v>
+      </c>
+      <c r="F12" t="n">
+        <v>140</v>
+      </c>
+      <c r="G12" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H12" t="n">
+        <v>111.111111</v>
+      </c>
+      <c r="I12" t="n">
+        <v>211.111111</v>
+      </c>
+      <c r="J12" t="n">
+        <v>113.429137</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" t="n">
+        <v>90.743309</v>
+      </c>
+      <c r="M12" t="n">
+        <v>5160</v>
+      </c>
+      <c r="N12" t="n">
+        <v>88.88888900000001</v>
+      </c>
+      <c r="O12" t="n">
+        <v>528.8888889999999</v>
+      </c>
+      <c r="P12" t="n">
+        <v>2000</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>111.111111</v>
+      </c>
+      <c r="R12" t="n">
+        <v>80</v>
+      </c>
+      <c r="S12" t="n">
+        <v>9.57131</v>
+      </c>
+      <c r="T12" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>M3</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>FY1</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>-0.994957</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.006997</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-0.100055</v>
+      </c>
+      <c r="F13" t="n">
+        <v>140</v>
+      </c>
+      <c r="G13" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H13" t="n">
+        <v>111.111111</v>
+      </c>
+      <c r="I13" t="n">
+        <v>211.111111</v>
+      </c>
+      <c r="J13" t="n">
+        <v>113.429137</v>
+      </c>
+      <c r="K13" t="n">
+        <v>2</v>
+      </c>
+      <c r="L13" t="n">
+        <v>91.743309</v>
+      </c>
+      <c r="M13" t="n">
+        <v>5020.705984</v>
+      </c>
+      <c r="N13" t="n">
+        <v>89.868453</v>
+      </c>
+      <c r="O13" t="n">
+        <v>514.881122</v>
+      </c>
+      <c r="P13" t="n">
+        <v>2000</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>111.111111</v>
+      </c>
+      <c r="R13" t="n">
+        <v>80</v>
+      </c>
+      <c r="S13" t="n">
+        <v>9.420788</v>
+      </c>
+      <c r="T13" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>M3</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>FY5</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>-0.977469</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.187595</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-0.09676</v>
+      </c>
+      <c r="F14" t="n">
+        <v>140</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H14" t="n">
+        <v>111.111111</v>
+      </c>
+      <c r="I14" t="n">
+        <v>211.111111</v>
+      </c>
+      <c r="J14" t="n">
+        <v>80.382526</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" t="n">
+        <v>64.306021</v>
+      </c>
+      <c r="M14" t="n">
+        <v>4200</v>
+      </c>
+      <c r="N14" t="n">
+        <v>-311.111111</v>
+      </c>
+      <c r="O14" t="n">
+        <v>428.888889</v>
+      </c>
+      <c r="P14" t="n">
+        <v>2000</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>111.111111</v>
+      </c>
+      <c r="R14" t="n">
+        <v>80</v>
+      </c>
+      <c r="S14" t="n">
+        <v>8.438117</v>
+      </c>
+      <c r="T14" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>M3</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>FY5</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>-0.977469</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.187595</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-0.09676</v>
+      </c>
+      <c r="F15" t="n">
+        <v>140</v>
+      </c>
+      <c r="G15" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H15" t="n">
+        <v>111.111111</v>
+      </c>
+      <c r="I15" t="n">
+        <v>211.111111</v>
+      </c>
+      <c r="J15" t="n">
+        <v>80.382526</v>
+      </c>
+      <c r="K15" t="n">
+        <v>2</v>
+      </c>
+      <c r="L15" t="n">
+        <v>65.306021</v>
+      </c>
+      <c r="M15" t="n">
+        <v>4063.154338</v>
+      </c>
+      <c r="N15" t="n">
+        <v>-284.847802</v>
+      </c>
+      <c r="O15" t="n">
+        <v>415.342551</v>
+      </c>
+      <c r="P15" t="n">
+        <v>2000</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>111.111111</v>
+      </c>
+      <c r="R15" t="n">
+        <v>80</v>
+      </c>
+      <c r="S15" t="n">
+        <v>8.272681</v>
+      </c>
+      <c r="T15" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>M3</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>FY5</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>-0.977469</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.187595</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-0.09676</v>
+      </c>
+      <c r="F16" t="n">
+        <v>140</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H16" t="n">
+        <v>111.111111</v>
+      </c>
+      <c r="I16" t="n">
+        <v>211.111111</v>
+      </c>
+      <c r="J16" t="n">
+        <v>80.382526</v>
+      </c>
+      <c r="K16" t="n">
+        <v>3</v>
+      </c>
+      <c r="L16" t="n">
+        <v>66.306021</v>
+      </c>
+      <c r="M16" t="n">
+        <v>3926.308675</v>
+      </c>
+      <c r="N16" t="n">
+        <v>-258.584493</v>
+      </c>
+      <c r="O16" t="n">
+        <v>401.796212</v>
+      </c>
+      <c r="P16" t="n">
+        <v>2000</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>111.111111</v>
+      </c>
+      <c r="R16" t="n">
+        <v>80</v>
+      </c>
+      <c r="S16" t="n">
+        <v>8.103869</v>
+      </c>
+      <c r="T16" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
+      <c r="T17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>性能指标摘要</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
+      <c r="T19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>总遮蔽时间(s)</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>75.000000</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>总烟幕弹数量</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>15.000000</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>平均遮蔽时间(s)</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>25.000000</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr"/>
+      <c r="T22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>效率指标</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>5.000000</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr"/>
+      <c r="T23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: Add smoke optimization script and update results
Co-authored-by: 3349523701 <3349523701@qq.com>
</commit_message>
<xml_diff>
--- a/结果3.xlsx
+++ b/结果3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -547,58 +547,58 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-0.9948</v>
+        <v>-0.99476</v>
       </c>
       <c r="D2" t="n">
-        <v>0.011803</v>
+        <v>0.012181</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.101166</v>
+        <v>-0.101506</v>
       </c>
       <c r="F2" t="n">
         <v>140</v>
       </c>
       <c r="G2" t="n">
-        <v>6000</v>
+        <v>8000</v>
       </c>
       <c r="H2" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="I2" t="n">
-        <v>600</v>
+        <v>800</v>
       </c>
       <c r="J2" t="n">
-        <v>84.72633</v>
+        <v>70.368708</v>
       </c>
       <c r="K2" t="n">
         <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>67.781064</v>
+        <v>49.258096</v>
       </c>
       <c r="M2" t="n">
-        <v>8360</v>
+        <v>10940</v>
       </c>
       <c r="N2" t="n">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="O2" t="n">
-        <v>840</v>
+        <v>1100</v>
       </c>
       <c r="P2" t="n">
-        <v>6000</v>
+        <v>8000</v>
       </c>
       <c r="Q2" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="R2" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="S2" t="n">
-        <v>80.816728</v>
+        <v>51.258096</v>
       </c>
       <c r="T2" t="n">
-        <v>5.542853</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="3">
@@ -613,58 +613,58 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-0.9948</v>
+        <v>-0.99476</v>
       </c>
       <c r="D3" t="n">
-        <v>0.011803</v>
+        <v>0.012181</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.101166</v>
+        <v>-0.101506</v>
       </c>
       <c r="F3" t="n">
         <v>140</v>
       </c>
       <c r="G3" t="n">
-        <v>6000</v>
+        <v>8000</v>
       </c>
       <c r="H3" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="I3" t="n">
-        <v>600</v>
+        <v>800</v>
       </c>
       <c r="J3" t="n">
-        <v>84.72633</v>
+        <v>70.368708</v>
       </c>
       <c r="K3" t="n">
         <v>2</v>
       </c>
       <c r="L3" t="n">
-        <v>68.981064</v>
+        <v>56.294967</v>
       </c>
       <c r="M3" t="n">
-        <v>8192.873677</v>
+        <v>9960</v>
       </c>
       <c r="N3" t="n">
-        <v>113.982855</v>
+        <v>96</v>
       </c>
       <c r="O3" t="n">
-        <v>823.004103</v>
+        <v>1000</v>
       </c>
       <c r="P3" t="n">
-        <v>6000</v>
+        <v>8000</v>
       </c>
       <c r="Q3" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="R3" t="n">
         <v>80</v>
       </c>
       <c r="S3" t="n">
-        <v>81.795019</v>
+        <v>58.294967</v>
       </c>
       <c r="T3" t="n">
-        <v>6.497891</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="4">
@@ -679,64 +679,64 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.9948</v>
+        <v>-0.99476</v>
       </c>
       <c r="D4" t="n">
-        <v>0.011803</v>
+        <v>0.012181</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.101166</v>
+        <v>-0.101506</v>
       </c>
       <c r="F4" t="n">
         <v>140</v>
       </c>
       <c r="G4" t="n">
-        <v>6000</v>
+        <v>8000</v>
       </c>
       <c r="H4" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="I4" t="n">
-        <v>600</v>
+        <v>800</v>
       </c>
       <c r="J4" t="n">
-        <v>84.72633</v>
+        <v>70.368708</v>
       </c>
       <c r="K4" t="n">
         <v>3</v>
       </c>
       <c r="L4" t="n">
-        <v>70.18106400000001</v>
+        <v>63.331837</v>
       </c>
       <c r="M4" t="n">
-        <v>8025.747354</v>
+        <v>8980</v>
       </c>
       <c r="N4" t="n">
-        <v>115.965709</v>
+        <v>108</v>
       </c>
       <c r="O4" t="n">
-        <v>806.008206</v>
+        <v>900</v>
       </c>
       <c r="P4" t="n">
-        <v>6000</v>
+        <v>8000</v>
       </c>
       <c r="Q4" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="R4" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="S4" t="n">
-        <v>82.769245</v>
+        <v>65.33183699999999</v>
       </c>
       <c r="T4" t="n">
-        <v>6.379775</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>M2</t>
+          <t>M1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -745,64 +745,64 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.978548</v>
+        <v>-0.960422</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.167751</v>
+        <v>-0.243947</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.1196</v>
+        <v>-0.134459</v>
       </c>
       <c r="F5" t="n">
         <v>140</v>
       </c>
       <c r="G5" t="n">
-        <v>5700</v>
+        <v>7000</v>
       </c>
       <c r="H5" t="n">
-        <v>320</v>
+        <v>130</v>
       </c>
       <c r="I5" t="n">
-        <v>630</v>
+        <v>700</v>
       </c>
       <c r="J5" t="n">
-        <v>45.986522</v>
+        <v>37.186033</v>
       </c>
       <c r="K5" t="n">
         <v>1</v>
       </c>
       <c r="L5" t="n">
-        <v>36.789218</v>
+        <v>26.030223</v>
       </c>
       <c r="M5" t="n">
-        <v>6960</v>
+        <v>8500</v>
       </c>
       <c r="N5" t="n">
-        <v>536</v>
+        <v>511</v>
       </c>
       <c r="O5" t="n">
-        <v>784</v>
+        <v>910</v>
       </c>
       <c r="P5" t="n">
-        <v>5700</v>
+        <v>7000</v>
       </c>
       <c r="Q5" t="n">
-        <v>320</v>
+        <v>130</v>
       </c>
       <c r="R5" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="S5" t="n">
-        <v>49.360435</v>
+        <v>28.030223</v>
       </c>
       <c r="T5" t="n">
-        <v>5.752558</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>M2</t>
+          <t>M1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -811,58 +811,58 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-0.978548</v>
+        <v>-0.960422</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.167751</v>
+        <v>-0.243947</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.1196</v>
+        <v>-0.134459</v>
       </c>
       <c r="F6" t="n">
         <v>140</v>
       </c>
       <c r="G6" t="n">
-        <v>5700</v>
+        <v>7000</v>
       </c>
       <c r="H6" t="n">
-        <v>320</v>
+        <v>130</v>
       </c>
       <c r="I6" t="n">
-        <v>630</v>
+        <v>700</v>
       </c>
       <c r="J6" t="n">
-        <v>45.986522</v>
+        <v>37.186033</v>
       </c>
       <c r="K6" t="n">
         <v>2</v>
       </c>
       <c r="L6" t="n">
-        <v>37.989218</v>
+        <v>29.748826</v>
       </c>
       <c r="M6" t="n">
-        <v>6795.604006</v>
+        <v>8000</v>
       </c>
       <c r="N6" t="n">
-        <v>507.81783</v>
+        <v>384</v>
       </c>
       <c r="O6" t="n">
-        <v>763.907156</v>
+        <v>840</v>
       </c>
       <c r="P6" t="n">
-        <v>5700</v>
+        <v>7000</v>
       </c>
       <c r="Q6" t="n">
-        <v>320</v>
+        <v>130</v>
       </c>
       <c r="R6" t="n">
         <v>80</v>
       </c>
       <c r="S6" t="n">
-        <v>50.303315</v>
+        <v>31.748826</v>
       </c>
       <c r="T6" t="n">
-        <v>6.548749</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="7">
@@ -873,20 +873,20 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>FY2</t>
+          <t>FY3</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.978548</v>
+        <v>-0.089975</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.167751</v>
+        <v>0.995723</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.1196</v>
+        <v>-0.020994</v>
       </c>
       <c r="F7" t="n">
-        <v>140</v>
+        <v>87.193557</v>
       </c>
       <c r="G7" t="n">
         <v>5700</v>
@@ -898,22 +898,22 @@
         <v>630</v>
       </c>
       <c r="J7" t="n">
-        <v>45.986522</v>
+        <v>38.23977</v>
       </c>
       <c r="K7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L7" t="n">
-        <v>39.189218</v>
+        <v>26.767839</v>
       </c>
       <c r="M7" t="n">
-        <v>6631.208012</v>
+        <v>5790</v>
       </c>
       <c r="N7" t="n">
-        <v>479.635659</v>
+        <v>-676</v>
       </c>
       <c r="O7" t="n">
-        <v>743.814313</v>
+        <v>651</v>
       </c>
       <c r="P7" t="n">
         <v>5700</v>
@@ -922,151 +922,151 @@
         <v>320</v>
       </c>
       <c r="R7" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="S7" t="n">
-        <v>51.240473</v>
+        <v>28.767839</v>
       </c>
       <c r="T7" t="n">
-        <v>6.426534</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>M3</t>
+          <t>M2</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>FY4</t>
+          <t>FY3</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.9202050000000001</v>
+        <v>-0.089975</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.335218</v>
+        <v>0.995723</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.202117</v>
+        <v>-0.020994</v>
       </c>
       <c r="F8" t="n">
-        <v>140</v>
+        <v>87.193557</v>
       </c>
       <c r="G8" t="n">
-        <v>5400</v>
+        <v>5700</v>
       </c>
       <c r="H8" t="n">
-        <v>-40</v>
+        <v>320</v>
       </c>
       <c r="I8" t="n">
-        <v>570</v>
+        <v>630</v>
       </c>
       <c r="J8" t="n">
-        <v>43.468555</v>
+        <v>38.23977</v>
       </c>
       <c r="K8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L8" t="n">
-        <v>34.774844</v>
+        <v>30.591816</v>
       </c>
       <c r="M8" t="n">
-        <v>6520</v>
+        <v>5760</v>
       </c>
       <c r="N8" t="n">
-        <v>368</v>
+        <v>-344</v>
       </c>
       <c r="O8" t="n">
-        <v>816</v>
+        <v>644</v>
       </c>
       <c r="P8" t="n">
-        <v>5400</v>
+        <v>5700</v>
       </c>
       <c r="Q8" t="n">
-        <v>-40</v>
+        <v>320</v>
       </c>
       <c r="R8" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="S8" t="n">
-        <v>47.6136</v>
+        <v>32.591816</v>
       </c>
       <c r="T8" t="n">
-        <v>5.702962</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>M3</t>
+          <t>M2</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>FY4</t>
+          <t>FY3</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.9202050000000001</v>
+        <v>-0.089975</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.335218</v>
+        <v>0.995723</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.202117</v>
+        <v>-0.020994</v>
       </c>
       <c r="F9" t="n">
-        <v>140</v>
+        <v>87.193557</v>
       </c>
       <c r="G9" t="n">
-        <v>5400</v>
+        <v>5700</v>
       </c>
       <c r="H9" t="n">
-        <v>-40</v>
+        <v>320</v>
       </c>
       <c r="I9" t="n">
-        <v>570</v>
+        <v>630</v>
       </c>
       <c r="J9" t="n">
-        <v>43.468555</v>
+        <v>38.23977</v>
       </c>
       <c r="K9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L9" t="n">
-        <v>35.974844</v>
+        <v>34.415793</v>
       </c>
       <c r="M9" t="n">
-        <v>6365.40549</v>
+        <v>5730</v>
       </c>
       <c r="N9" t="n">
-        <v>311.683429</v>
+        <v>-12</v>
       </c>
       <c r="O9" t="n">
-        <v>782.0444199999999</v>
+        <v>637</v>
       </c>
       <c r="P9" t="n">
-        <v>5400</v>
+        <v>5700</v>
       </c>
       <c r="Q9" t="n">
-        <v>-40</v>
+        <v>320</v>
       </c>
       <c r="R9" t="n">
         <v>80</v>
       </c>
       <c r="S9" t="n">
-        <v>48.444572</v>
+        <v>36.415793</v>
       </c>
       <c r="T9" t="n">
-        <v>5.96186</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>M3</t>
+          <t>M2</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1075,58 +1075,322 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.9202050000000001</v>
+        <v>-0.946773</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.335218</v>
+        <v>-0.257522</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.202117</v>
+        <v>-0.193142</v>
       </c>
       <c r="F10" t="n">
         <v>140</v>
       </c>
       <c r="G10" t="n">
-        <v>5400</v>
+        <v>4750</v>
       </c>
       <c r="H10" t="n">
-        <v>-40</v>
+        <v>300</v>
       </c>
       <c r="I10" t="n">
-        <v>570</v>
+        <v>525</v>
       </c>
       <c r="J10" t="n">
-        <v>43.468555</v>
+        <v>47.152664</v>
       </c>
       <c r="K10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" t="n">
+        <v>33.006865</v>
+      </c>
+      <c r="M10" t="n">
+        <v>6625</v>
+      </c>
+      <c r="N10" t="n">
+        <v>810</v>
+      </c>
+      <c r="O10" t="n">
+        <v>907.5</v>
+      </c>
+      <c r="P10" t="n">
+        <v>4750</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>300</v>
+      </c>
+      <c r="R10" t="n">
+        <v>80</v>
+      </c>
+      <c r="S10" t="n">
+        <v>35.006865</v>
+      </c>
+      <c r="T10" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>M2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>FY4</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>-0.946773</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-0.257522</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-0.193142</v>
+      </c>
+      <c r="F11" t="n">
+        <v>140</v>
+      </c>
+      <c r="G11" t="n">
+        <v>4750</v>
+      </c>
+      <c r="H11" t="n">
+        <v>300</v>
+      </c>
+      <c r="I11" t="n">
+        <v>525</v>
+      </c>
+      <c r="J11" t="n">
+        <v>47.152664</v>
+      </c>
+      <c r="K11" t="n">
+        <v>2</v>
+      </c>
+      <c r="L11" t="n">
+        <v>37.722131</v>
+      </c>
+      <c r="M11" t="n">
+        <v>6000</v>
+      </c>
+      <c r="N11" t="n">
+        <v>640</v>
+      </c>
+      <c r="O11" t="n">
+        <v>780</v>
+      </c>
+      <c r="P11" t="n">
+        <v>4750</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>300</v>
+      </c>
+      <c r="R11" t="n">
+        <v>80</v>
+      </c>
+      <c r="S11" t="n">
+        <v>39.722131</v>
+      </c>
+      <c r="T11" t="n">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>M3</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>FY5</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>-0.972812</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.211121</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-0.095211</v>
+      </c>
+      <c r="F12" t="n">
+        <v>140</v>
+      </c>
+      <c r="G12" t="n">
+        <v>3600</v>
+      </c>
+      <c r="H12" t="n">
+        <v>40</v>
+      </c>
+      <c r="I12" t="n">
+        <v>380</v>
+      </c>
+      <c r="J12" t="n">
+        <v>69.01937</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" t="n">
+        <v>48.313559</v>
+      </c>
+      <c r="M12" t="n">
+        <v>6420</v>
+      </c>
+      <c r="N12" t="n">
+        <v>-572</v>
+      </c>
+      <c r="O12" t="n">
+        <v>656</v>
+      </c>
+      <c r="P12" t="n">
+        <v>3600</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>40</v>
+      </c>
+      <c r="R12" t="n">
+        <v>80</v>
+      </c>
+      <c r="S12" t="n">
+        <v>50.313559</v>
+      </c>
+      <c r="T12" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>M3</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>FY5</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>-0.972812</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.211121</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-0.095211</v>
+      </c>
+      <c r="F13" t="n">
+        <v>140</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3600</v>
+      </c>
+      <c r="H13" t="n">
+        <v>40</v>
+      </c>
+      <c r="I13" t="n">
+        <v>380</v>
+      </c>
+      <c r="J13" t="n">
+        <v>69.01937</v>
+      </c>
+      <c r="K13" t="n">
+        <v>2</v>
+      </c>
+      <c r="L13" t="n">
+        <v>55.215496</v>
+      </c>
+      <c r="M13" t="n">
+        <v>5480</v>
+      </c>
+      <c r="N13" t="n">
+        <v>-368</v>
+      </c>
+      <c r="O13" t="n">
+        <v>564</v>
+      </c>
+      <c r="P13" t="n">
+        <v>3600</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>40</v>
+      </c>
+      <c r="R13" t="n">
+        <v>80</v>
+      </c>
+      <c r="S13" t="n">
+        <v>57.215496</v>
+      </c>
+      <c r="T13" t="n">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>M3</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>FY5</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>-0.972812</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.211121</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-0.095211</v>
+      </c>
+      <c r="F14" t="n">
+        <v>140</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3600</v>
+      </c>
+      <c r="H14" t="n">
+        <v>40</v>
+      </c>
+      <c r="I14" t="n">
+        <v>380</v>
+      </c>
+      <c r="J14" t="n">
+        <v>69.01937</v>
+      </c>
+      <c r="K14" t="n">
         <v>3</v>
       </c>
-      <c r="L10" t="n">
-        <v>37.174844</v>
-      </c>
-      <c r="M10" t="n">
-        <v>6210.810981</v>
-      </c>
-      <c r="N10" t="n">
-        <v>255.366857</v>
-      </c>
-      <c r="O10" t="n">
-        <v>748.08884</v>
-      </c>
-      <c r="P10" t="n">
-        <v>5400</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>-40</v>
-      </c>
-      <c r="R10" t="n">
-        <v>90</v>
-      </c>
-      <c r="S10" t="n">
-        <v>49.263798</v>
-      </c>
-      <c r="T10" t="n">
-        <v>6.237945</v>
+      <c r="L14" t="n">
+        <v>62.117433</v>
+      </c>
+      <c r="M14" t="n">
+        <v>4540</v>
+      </c>
+      <c r="N14" t="n">
+        <v>-164</v>
+      </c>
+      <c r="O14" t="n">
+        <v>472</v>
+      </c>
+      <c r="P14" t="n">
+        <v>3600</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>40</v>
+      </c>
+      <c r="R14" t="n">
+        <v>80</v>
+      </c>
+      <c r="S14" t="n">
+        <v>64.11743300000001</v>
+      </c>
+      <c r="T14" t="n">
+        <v>1.32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Implement final correct optimization for smoke deployment
Co-authored-by: 3349523701 <3349523701@qq.com>
</commit_message>
<xml_diff>
--- a/结果3.xlsx
+++ b/结果3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,7 +556,7 @@
         <v>-0.101506</v>
       </c>
       <c r="F2" t="n">
-        <v>140</v>
+        <v>91</v>
       </c>
       <c r="G2" t="n">
         <v>8000</v>
@@ -568,22 +568,22 @@
         <v>800</v>
       </c>
       <c r="J2" t="n">
-        <v>70.368708</v>
+        <v>108.259551</v>
       </c>
       <c r="K2" t="n">
         <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>49.258096</v>
+        <v>81.19466300000001</v>
       </c>
       <c r="M2" t="n">
-        <v>10940</v>
+        <v>10450</v>
       </c>
       <c r="N2" t="n">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="O2" t="n">
-        <v>1100</v>
+        <v>1050</v>
       </c>
       <c r="P2" t="n">
         <v>8000</v>
@@ -592,13 +592,13 @@
         <v>120</v>
       </c>
       <c r="R2" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="S2" t="n">
-        <v>51.258096</v>
+        <v>108.759551</v>
       </c>
       <c r="T2" t="n">
-        <v>1.2</v>
+        <v>4.611044</v>
       </c>
     </row>
     <row r="3">
@@ -622,7 +622,7 @@
         <v>-0.101506</v>
       </c>
       <c r="F3" t="n">
-        <v>140</v>
+        <v>91</v>
       </c>
       <c r="G3" t="n">
         <v>8000</v>
@@ -634,22 +634,22 @@
         <v>800</v>
       </c>
       <c r="J3" t="n">
-        <v>70.368708</v>
+        <v>108.259551</v>
       </c>
       <c r="K3" t="n">
         <v>2</v>
       </c>
       <c r="L3" t="n">
-        <v>56.294967</v>
+        <v>92.020618</v>
       </c>
       <c r="M3" t="n">
-        <v>9960</v>
+        <v>9470</v>
       </c>
       <c r="N3" t="n">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="O3" t="n">
-        <v>1000</v>
+        <v>950</v>
       </c>
       <c r="P3" t="n">
         <v>8000</v>
@@ -658,85 +658,85 @@
         <v>120</v>
       </c>
       <c r="R3" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="S3" t="n">
-        <v>58.294967</v>
+        <v>108.759551</v>
       </c>
       <c r="T3" t="n">
-        <v>1.26</v>
+        <v>3.47636</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>M1</t>
+          <t>M2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>FY1</t>
+          <t>FY2</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.99476</v>
+        <v>-0.97372</v>
       </c>
       <c r="D4" t="n">
-        <v>0.012181</v>
+        <v>-0.192924</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.101506</v>
+        <v>-0.121033</v>
       </c>
       <c r="F4" t="n">
-        <v>140</v>
+        <v>98</v>
       </c>
       <c r="G4" t="n">
-        <v>8000</v>
+        <v>6650</v>
       </c>
       <c r="H4" t="n">
-        <v>120</v>
+        <v>340</v>
       </c>
       <c r="I4" t="n">
-        <v>800</v>
+        <v>735</v>
       </c>
       <c r="J4" t="n">
-        <v>70.368708</v>
+        <v>56.065207</v>
       </c>
       <c r="K4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>63.331837</v>
+        <v>39.245645</v>
       </c>
       <c r="M4" t="n">
-        <v>8980</v>
+        <v>8255</v>
       </c>
       <c r="N4" t="n">
-        <v>108</v>
+        <v>658</v>
       </c>
       <c r="O4" t="n">
-        <v>900</v>
+        <v>934.5</v>
       </c>
       <c r="P4" t="n">
-        <v>8000</v>
+        <v>6650</v>
       </c>
       <c r="Q4" t="n">
-        <v>120</v>
+        <v>340</v>
       </c>
       <c r="R4" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="S4" t="n">
-        <v>65.33183699999999</v>
+        <v>56.565207</v>
       </c>
       <c r="T4" t="n">
-        <v>1.32</v>
+        <v>5.260544</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>M1</t>
+          <t>M2</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -745,64 +745,64 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.960422</v>
+        <v>-0.97372</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.243947</v>
+        <v>-0.192924</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.134459</v>
+        <v>-0.121033</v>
       </c>
       <c r="F5" t="n">
-        <v>140</v>
+        <v>98</v>
       </c>
       <c r="G5" t="n">
-        <v>7000</v>
+        <v>6650</v>
       </c>
       <c r="H5" t="n">
-        <v>130</v>
+        <v>340</v>
       </c>
       <c r="I5" t="n">
-        <v>700</v>
+        <v>735</v>
       </c>
       <c r="J5" t="n">
-        <v>37.186033</v>
+        <v>56.065207</v>
       </c>
       <c r="K5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L5" t="n">
-        <v>26.030223</v>
+        <v>44.852166</v>
       </c>
       <c r="M5" t="n">
-        <v>8500</v>
+        <v>7720</v>
       </c>
       <c r="N5" t="n">
-        <v>511</v>
+        <v>552</v>
       </c>
       <c r="O5" t="n">
-        <v>910</v>
+        <v>868</v>
       </c>
       <c r="P5" t="n">
-        <v>7000</v>
+        <v>6650</v>
       </c>
       <c r="Q5" t="n">
-        <v>130</v>
+        <v>340</v>
       </c>
       <c r="R5" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="S5" t="n">
-        <v>28.030223</v>
+        <v>56.565207</v>
       </c>
       <c r="T5" t="n">
-        <v>1.2</v>
+        <v>4.234165</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>M1</t>
+          <t>M2</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -811,64 +811,64 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-0.960422</v>
+        <v>-0.97372</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.243947</v>
+        <v>-0.192924</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.134459</v>
+        <v>-0.121033</v>
       </c>
       <c r="F6" t="n">
-        <v>140</v>
+        <v>98</v>
       </c>
       <c r="G6" t="n">
-        <v>7000</v>
+        <v>6650</v>
       </c>
       <c r="H6" t="n">
-        <v>130</v>
+        <v>340</v>
       </c>
       <c r="I6" t="n">
-        <v>700</v>
+        <v>735</v>
       </c>
       <c r="J6" t="n">
-        <v>37.186033</v>
+        <v>56.065207</v>
       </c>
       <c r="K6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L6" t="n">
-        <v>29.748826</v>
+        <v>50.458687</v>
       </c>
       <c r="M6" t="n">
-        <v>8000</v>
+        <v>7185</v>
       </c>
       <c r="N6" t="n">
-        <v>384</v>
+        <v>446</v>
       </c>
       <c r="O6" t="n">
-        <v>840</v>
+        <v>801.5</v>
       </c>
       <c r="P6" t="n">
-        <v>7000</v>
+        <v>6650</v>
       </c>
       <c r="Q6" t="n">
-        <v>130</v>
+        <v>340</v>
       </c>
       <c r="R6" t="n">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="S6" t="n">
-        <v>31.748826</v>
+        <v>56.565207</v>
       </c>
       <c r="T6" t="n">
-        <v>1.26</v>
+        <v>3.746194</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>M2</t>
+          <t>M3</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -877,64 +877,64 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.089975</v>
+        <v>-0.198479</v>
       </c>
       <c r="D7" t="n">
-        <v>0.995723</v>
+        <v>0.9791609999999999</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.020994</v>
+        <v>-0.043004</v>
       </c>
       <c r="F7" t="n">
-        <v>87.193557</v>
+        <v>81.10075000000001</v>
       </c>
       <c r="G7" t="n">
-        <v>5700</v>
+        <v>5400</v>
       </c>
       <c r="H7" t="n">
-        <v>320</v>
+        <v>-40</v>
       </c>
       <c r="I7" t="n">
-        <v>630</v>
+        <v>570</v>
       </c>
       <c r="J7" t="n">
-        <v>38.23977</v>
+        <v>37.274566</v>
       </c>
       <c r="K7" t="n">
         <v>1</v>
       </c>
       <c r="L7" t="n">
-        <v>26.767839</v>
+        <v>27.955924</v>
       </c>
       <c r="M7" t="n">
-        <v>5790</v>
+        <v>5550</v>
       </c>
       <c r="N7" t="n">
-        <v>-676</v>
+        <v>-780</v>
       </c>
       <c r="O7" t="n">
-        <v>651</v>
+        <v>602.5</v>
       </c>
       <c r="P7" t="n">
-        <v>5700</v>
+        <v>5400</v>
       </c>
       <c r="Q7" t="n">
-        <v>320</v>
+        <v>-40</v>
       </c>
       <c r="R7" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="S7" t="n">
-        <v>28.767839</v>
+        <v>37.774566</v>
       </c>
       <c r="T7" t="n">
-        <v>1.2</v>
+        <v>4.895187</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>M2</t>
+          <t>M3</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -943,124 +943,124 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.089975</v>
+        <v>-0.198479</v>
       </c>
       <c r="D8" t="n">
-        <v>0.995723</v>
+        <v>0.9791609999999999</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.020994</v>
+        <v>-0.043004</v>
       </c>
       <c r="F8" t="n">
-        <v>87.193557</v>
+        <v>81.10075000000001</v>
       </c>
       <c r="G8" t="n">
-        <v>5700</v>
+        <v>5400</v>
       </c>
       <c r="H8" t="n">
-        <v>320</v>
+        <v>-40</v>
       </c>
       <c r="I8" t="n">
-        <v>630</v>
+        <v>570</v>
       </c>
       <c r="J8" t="n">
-        <v>38.23977</v>
+        <v>37.274566</v>
       </c>
       <c r="K8" t="n">
         <v>2</v>
       </c>
       <c r="L8" t="n">
-        <v>30.591816</v>
+        <v>31.683381</v>
       </c>
       <c r="M8" t="n">
-        <v>5760</v>
+        <v>5490</v>
       </c>
       <c r="N8" t="n">
-        <v>-344</v>
+        <v>-484</v>
       </c>
       <c r="O8" t="n">
-        <v>644</v>
+        <v>589.5</v>
       </c>
       <c r="P8" t="n">
-        <v>5700</v>
+        <v>5400</v>
       </c>
       <c r="Q8" t="n">
-        <v>320</v>
+        <v>-40</v>
       </c>
       <c r="R8" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="S8" t="n">
-        <v>32.591816</v>
+        <v>37.774566</v>
       </c>
       <c r="T8" t="n">
-        <v>1.26</v>
+        <v>4.51467</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>M2</t>
+          <t>M1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>FY3</t>
+          <t>FY4</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.089975</v>
+        <v>-0.93576</v>
       </c>
       <c r="D9" t="n">
-        <v>0.995723</v>
+        <v>-0.288526</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.020994</v>
+        <v>-0.202748</v>
       </c>
       <c r="F9" t="n">
-        <v>87.193557</v>
+        <v>112</v>
       </c>
       <c r="G9" t="n">
-        <v>5700</v>
+        <v>5000</v>
       </c>
       <c r="H9" t="n">
-        <v>320</v>
+        <v>150</v>
       </c>
       <c r="I9" t="n">
-        <v>630</v>
+        <v>500</v>
       </c>
       <c r="J9" t="n">
-        <v>38.23977</v>
+        <v>57.249134</v>
       </c>
       <c r="K9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L9" t="n">
-        <v>34.415793</v>
+        <v>45.799307</v>
       </c>
       <c r="M9" t="n">
-        <v>5730</v>
+        <v>6200</v>
       </c>
       <c r="N9" t="n">
-        <v>-12</v>
+        <v>520</v>
       </c>
       <c r="O9" t="n">
-        <v>637</v>
+        <v>760</v>
       </c>
       <c r="P9" t="n">
-        <v>5700</v>
+        <v>5000</v>
       </c>
       <c r="Q9" t="n">
-        <v>320</v>
+        <v>150</v>
       </c>
       <c r="R9" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="S9" t="n">
-        <v>36.415793</v>
+        <v>57.749134</v>
       </c>
       <c r="T9" t="n">
-        <v>1.32</v>
+        <v>5.204866</v>
       </c>
     </row>
     <row r="10">
@@ -1071,326 +1071,62 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>FY4</t>
+          <t>FY5</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.946773</v>
+        <v>-0.96648</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.257522</v>
+        <v>0.239519</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.193142</v>
+        <v>-0.092446</v>
       </c>
       <c r="F10" t="n">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="G10" t="n">
-        <v>4750</v>
+        <v>3800</v>
       </c>
       <c r="H10" t="n">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="I10" t="n">
-        <v>525</v>
+        <v>420</v>
       </c>
       <c r="J10" t="n">
-        <v>47.152664</v>
+        <v>79.992232</v>
       </c>
       <c r="K10" t="n">
         <v>1</v>
       </c>
       <c r="L10" t="n">
-        <v>33.006865</v>
+        <v>63.993785</v>
       </c>
       <c r="M10" t="n">
-        <v>6625</v>
+        <v>5640</v>
       </c>
       <c r="N10" t="n">
-        <v>810</v>
+        <v>-176</v>
       </c>
       <c r="O10" t="n">
-        <v>907.5</v>
+        <v>596</v>
       </c>
       <c r="P10" t="n">
-        <v>4750</v>
+        <v>3800</v>
       </c>
       <c r="Q10" t="n">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="R10" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="S10" t="n">
-        <v>35.006865</v>
+        <v>80.492232</v>
       </c>
       <c r="T10" t="n">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>M2</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>FY4</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>-0.946773</v>
-      </c>
-      <c r="D11" t="n">
-        <v>-0.257522</v>
-      </c>
-      <c r="E11" t="n">
-        <v>-0.193142</v>
-      </c>
-      <c r="F11" t="n">
-        <v>140</v>
-      </c>
-      <c r="G11" t="n">
-        <v>4750</v>
-      </c>
-      <c r="H11" t="n">
-        <v>300</v>
-      </c>
-      <c r="I11" t="n">
-        <v>525</v>
-      </c>
-      <c r="J11" t="n">
-        <v>47.152664</v>
-      </c>
-      <c r="K11" t="n">
-        <v>2</v>
-      </c>
-      <c r="L11" t="n">
-        <v>37.722131</v>
-      </c>
-      <c r="M11" t="n">
-        <v>6000</v>
-      </c>
-      <c r="N11" t="n">
-        <v>640</v>
-      </c>
-      <c r="O11" t="n">
-        <v>780</v>
-      </c>
-      <c r="P11" t="n">
-        <v>4750</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>300</v>
-      </c>
-      <c r="R11" t="n">
-        <v>80</v>
-      </c>
-      <c r="S11" t="n">
-        <v>39.722131</v>
-      </c>
-      <c r="T11" t="n">
-        <v>1.26</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>M3</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>FY5</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>-0.972812</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.211121</v>
-      </c>
-      <c r="E12" t="n">
-        <v>-0.095211</v>
-      </c>
-      <c r="F12" t="n">
-        <v>140</v>
-      </c>
-      <c r="G12" t="n">
-        <v>3600</v>
-      </c>
-      <c r="H12" t="n">
-        <v>40</v>
-      </c>
-      <c r="I12" t="n">
-        <v>380</v>
-      </c>
-      <c r="J12" t="n">
-        <v>69.01937</v>
-      </c>
-      <c r="K12" t="n">
-        <v>1</v>
-      </c>
-      <c r="L12" t="n">
-        <v>48.313559</v>
-      </c>
-      <c r="M12" t="n">
-        <v>6420</v>
-      </c>
-      <c r="N12" t="n">
-        <v>-572</v>
-      </c>
-      <c r="O12" t="n">
-        <v>656</v>
-      </c>
-      <c r="P12" t="n">
-        <v>3600</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>40</v>
-      </c>
-      <c r="R12" t="n">
-        <v>80</v>
-      </c>
-      <c r="S12" t="n">
-        <v>50.313559</v>
-      </c>
-      <c r="T12" t="n">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>M3</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>FY5</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>-0.972812</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.211121</v>
-      </c>
-      <c r="E13" t="n">
-        <v>-0.095211</v>
-      </c>
-      <c r="F13" t="n">
-        <v>140</v>
-      </c>
-      <c r="G13" t="n">
-        <v>3600</v>
-      </c>
-      <c r="H13" t="n">
-        <v>40</v>
-      </c>
-      <c r="I13" t="n">
-        <v>380</v>
-      </c>
-      <c r="J13" t="n">
-        <v>69.01937</v>
-      </c>
-      <c r="K13" t="n">
-        <v>2</v>
-      </c>
-      <c r="L13" t="n">
-        <v>55.215496</v>
-      </c>
-      <c r="M13" t="n">
-        <v>5480</v>
-      </c>
-      <c r="N13" t="n">
-        <v>-368</v>
-      </c>
-      <c r="O13" t="n">
-        <v>564</v>
-      </c>
-      <c r="P13" t="n">
-        <v>3600</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>40</v>
-      </c>
-      <c r="R13" t="n">
-        <v>80</v>
-      </c>
-      <c r="S13" t="n">
-        <v>57.215496</v>
-      </c>
-      <c r="T13" t="n">
-        <v>1.26</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>M3</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>FY5</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>-0.972812</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.211121</v>
-      </c>
-      <c r="E14" t="n">
-        <v>-0.095211</v>
-      </c>
-      <c r="F14" t="n">
-        <v>140</v>
-      </c>
-      <c r="G14" t="n">
-        <v>3600</v>
-      </c>
-      <c r="H14" t="n">
-        <v>40</v>
-      </c>
-      <c r="I14" t="n">
-        <v>380</v>
-      </c>
-      <c r="J14" t="n">
-        <v>69.01937</v>
-      </c>
-      <c r="K14" t="n">
-        <v>3</v>
-      </c>
-      <c r="L14" t="n">
-        <v>62.117433</v>
-      </c>
-      <c r="M14" t="n">
-        <v>4540</v>
-      </c>
-      <c r="N14" t="n">
-        <v>-164</v>
-      </c>
-      <c r="O14" t="n">
-        <v>472</v>
-      </c>
-      <c r="P14" t="n">
-        <v>3600</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>40</v>
-      </c>
-      <c r="R14" t="n">
-        <v>80</v>
-      </c>
-      <c r="S14" t="n">
-        <v>64.11743300000001</v>
-      </c>
-      <c r="T14" t="n">
-        <v>1.32</v>
+        <v>4.305364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Implement optimal smoke strategy and generate results
Co-authored-by: 3349523701 <3349523701@qq.com>
</commit_message>
<xml_diff>
--- a/结果3.xlsx
+++ b/结果3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -547,58 +547,58 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-0.99476</v>
+        <v>-0.994734</v>
       </c>
       <c r="D2" t="n">
-        <v>0.012181</v>
+        <v>0.012434</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.101506</v>
+        <v>-0.101734</v>
       </c>
       <c r="F2" t="n">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="G2" t="n">
-        <v>8000</v>
+        <v>9000</v>
       </c>
       <c r="H2" t="n">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="I2" t="n">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="J2" t="n">
-        <v>108.259551</v>
+        <v>104.077493</v>
       </c>
       <c r="K2" t="n">
         <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>81.19466300000001</v>
+        <v>67.65037100000001</v>
       </c>
       <c r="M2" t="n">
-        <v>10450</v>
+        <v>12080</v>
       </c>
       <c r="N2" t="n">
-        <v>90</v>
+        <v>71.5</v>
       </c>
       <c r="O2" t="n">
-        <v>1050</v>
+        <v>1215</v>
       </c>
       <c r="P2" t="n">
-        <v>8000</v>
+        <v>8980</v>
       </c>
       <c r="Q2" t="n">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="R2" t="n">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="S2" t="n">
-        <v>108.759551</v>
+        <v>105.312222</v>
       </c>
       <c r="T2" t="n">
-        <v>4.611044</v>
+        <v>1.69136</v>
       </c>
     </row>
     <row r="3">
@@ -613,124 +613,124 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-0.99476</v>
+        <v>-0.994734</v>
       </c>
       <c r="D3" t="n">
-        <v>0.012181</v>
+        <v>0.012434</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.101506</v>
+        <v>-0.101734</v>
       </c>
       <c r="F3" t="n">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="G3" t="n">
-        <v>8000</v>
+        <v>9000</v>
       </c>
       <c r="H3" t="n">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="I3" t="n">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="J3" t="n">
-        <v>108.259551</v>
+        <v>104.077493</v>
       </c>
       <c r="K3" t="n">
         <v>2</v>
       </c>
       <c r="L3" t="n">
-        <v>92.020618</v>
+        <v>78.05812</v>
       </c>
       <c r="M3" t="n">
-        <v>9470</v>
+        <v>11200</v>
       </c>
       <c r="N3" t="n">
-        <v>102</v>
+        <v>82.5</v>
       </c>
       <c r="O3" t="n">
-        <v>950</v>
+        <v>1125</v>
       </c>
       <c r="P3" t="n">
-        <v>8000</v>
+        <v>9000</v>
       </c>
       <c r="Q3" t="n">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="R3" t="n">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="S3" t="n">
-        <v>108.759551</v>
+        <v>105.077493</v>
       </c>
       <c r="T3" t="n">
-        <v>3.47636</v>
+        <v>1.346894</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>M2</t>
+          <t>M1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>FY2</t>
+          <t>FY1</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.97372</v>
+        <v>-0.994734</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.192924</v>
+        <v>0.012434</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.121033</v>
+        <v>-0.101734</v>
       </c>
       <c r="F4" t="n">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="G4" t="n">
-        <v>6650</v>
+        <v>9000</v>
       </c>
       <c r="H4" t="n">
-        <v>340</v>
+        <v>110</v>
       </c>
       <c r="I4" t="n">
-        <v>735</v>
+        <v>900</v>
       </c>
       <c r="J4" t="n">
-        <v>56.065207</v>
+        <v>104.077493</v>
       </c>
       <c r="K4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L4" t="n">
-        <v>39.245645</v>
+        <v>88.465869</v>
       </c>
       <c r="M4" t="n">
-        <v>8255</v>
+        <v>10320</v>
       </c>
       <c r="N4" t="n">
-        <v>658</v>
+        <v>93.5</v>
       </c>
       <c r="O4" t="n">
-        <v>934.5</v>
+        <v>1035</v>
       </c>
       <c r="P4" t="n">
-        <v>6650</v>
+        <v>9020</v>
       </c>
       <c r="Q4" t="n">
-        <v>340</v>
+        <v>125</v>
       </c>
       <c r="R4" t="n">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="S4" t="n">
-        <v>56.565207</v>
+        <v>104.844265</v>
       </c>
       <c r="T4" t="n">
-        <v>5.260544</v>
+        <v>1.205327</v>
       </c>
     </row>
     <row r="5">
@@ -745,58 +745,58 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.97372</v>
+        <v>-0.965804</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.192924</v>
+        <v>-0.228281</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.121033</v>
+        <v>-0.122921</v>
       </c>
       <c r="F5" t="n">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G5" t="n">
-        <v>6650</v>
+        <v>7600</v>
       </c>
       <c r="H5" t="n">
-        <v>340</v>
+        <v>360</v>
       </c>
       <c r="I5" t="n">
-        <v>735</v>
+        <v>840</v>
       </c>
       <c r="J5" t="n">
-        <v>56.065207</v>
+        <v>47.955658</v>
       </c>
       <c r="K5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L5" t="n">
-        <v>44.852166</v>
+        <v>31.171178</v>
       </c>
       <c r="M5" t="n">
-        <v>7720</v>
+        <v>9140</v>
       </c>
       <c r="N5" t="n">
-        <v>552</v>
+        <v>724</v>
       </c>
       <c r="O5" t="n">
-        <v>868</v>
+        <v>1036</v>
       </c>
       <c r="P5" t="n">
-        <v>6650</v>
+        <v>7580</v>
       </c>
       <c r="Q5" t="n">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="R5" t="n">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="S5" t="n">
-        <v>56.565207</v>
+        <v>49.199032</v>
       </c>
       <c r="T5" t="n">
-        <v>4.234165</v>
+        <v>1.911917</v>
       </c>
     </row>
     <row r="6">
@@ -811,124 +811,124 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-0.97372</v>
+        <v>-0.965804</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.192924</v>
+        <v>-0.228281</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.121033</v>
+        <v>-0.122921</v>
       </c>
       <c r="F6" t="n">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G6" t="n">
-        <v>6650</v>
+        <v>7600</v>
       </c>
       <c r="H6" t="n">
-        <v>340</v>
+        <v>360</v>
       </c>
       <c r="I6" t="n">
-        <v>735</v>
+        <v>840</v>
       </c>
       <c r="J6" t="n">
-        <v>56.065207</v>
+        <v>47.955658</v>
       </c>
       <c r="K6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L6" t="n">
-        <v>50.458687</v>
+        <v>35.966744</v>
       </c>
       <c r="M6" t="n">
-        <v>7185</v>
+        <v>8700</v>
       </c>
       <c r="N6" t="n">
-        <v>446</v>
+        <v>620</v>
       </c>
       <c r="O6" t="n">
-        <v>801.5</v>
+        <v>980</v>
       </c>
       <c r="P6" t="n">
-        <v>6650</v>
+        <v>7600</v>
       </c>
       <c r="Q6" t="n">
-        <v>340</v>
+        <v>360</v>
       </c>
       <c r="R6" t="n">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="S6" t="n">
-        <v>56.565207</v>
+        <v>51.808149</v>
       </c>
       <c r="T6" t="n">
-        <v>3.746194</v>
+        <v>1.621917</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>M3</t>
+          <t>M2</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>FY3</t>
+          <t>FY2</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.198479</v>
+        <v>-0.965804</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9791609999999999</v>
+        <v>-0.228281</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.043004</v>
+        <v>-0.122921</v>
       </c>
       <c r="F7" t="n">
-        <v>81.10075000000001</v>
+        <v>95</v>
       </c>
       <c r="G7" t="n">
-        <v>5400</v>
+        <v>7600</v>
       </c>
       <c r="H7" t="n">
-        <v>-40</v>
+        <v>360</v>
       </c>
       <c r="I7" t="n">
-        <v>570</v>
+        <v>840</v>
       </c>
       <c r="J7" t="n">
-        <v>37.274566</v>
+        <v>47.955658</v>
       </c>
       <c r="K7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L7" t="n">
-        <v>27.955924</v>
+        <v>40.762309</v>
       </c>
       <c r="M7" t="n">
-        <v>5550</v>
+        <v>8260</v>
       </c>
       <c r="N7" t="n">
-        <v>-780</v>
+        <v>516</v>
       </c>
       <c r="O7" t="n">
-        <v>602.5</v>
+        <v>924</v>
       </c>
       <c r="P7" t="n">
-        <v>5400</v>
+        <v>7620</v>
       </c>
       <c r="Q7" t="n">
-        <v>-40</v>
+        <v>375</v>
       </c>
       <c r="R7" t="n">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="S7" t="n">
-        <v>37.774566</v>
+        <v>56.085538</v>
       </c>
       <c r="T7" t="n">
-        <v>4.895187</v>
+        <v>1.281802</v>
       </c>
     </row>
     <row r="8">
@@ -943,190 +943,586 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.198479</v>
+        <v>0.102194</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9791609999999999</v>
+        <v>0.994693</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.043004</v>
+        <v>-0.011923</v>
       </c>
       <c r="F8" t="n">
-        <v>81.10075000000001</v>
+        <v>75</v>
       </c>
       <c r="G8" t="n">
-        <v>5400</v>
+        <v>6300</v>
       </c>
       <c r="H8" t="n">
-        <v>-40</v>
+        <v>-80</v>
       </c>
       <c r="I8" t="n">
-        <v>570</v>
+        <v>665</v>
       </c>
       <c r="J8" t="n">
-        <v>37.274566</v>
+        <v>39.141055</v>
       </c>
       <c r="K8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L8" t="n">
-        <v>31.683381</v>
+        <v>25.441686</v>
       </c>
       <c r="M8" t="n">
-        <v>5490</v>
+        <v>6195</v>
       </c>
       <c r="N8" t="n">
-        <v>-484</v>
+        <v>-1102</v>
       </c>
       <c r="O8" t="n">
-        <v>589.5</v>
+        <v>677.25</v>
       </c>
       <c r="P8" t="n">
-        <v>5400</v>
+        <v>6280</v>
       </c>
       <c r="Q8" t="n">
-        <v>-40</v>
+        <v>-95</v>
       </c>
       <c r="R8" t="n">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="S8" t="n">
-        <v>37.774566</v>
+        <v>39.917057</v>
       </c>
       <c r="T8" t="n">
-        <v>4.51467</v>
+        <v>2.238126</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>M1</t>
+          <t>M3</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>FY4</t>
+          <t>FY3</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.93576</v>
+        <v>0.102194</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.288526</v>
+        <v>0.994693</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.202748</v>
+        <v>-0.011923</v>
       </c>
       <c r="F9" t="n">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="G9" t="n">
-        <v>5000</v>
+        <v>6300</v>
       </c>
       <c r="H9" t="n">
-        <v>150</v>
+        <v>-80</v>
       </c>
       <c r="I9" t="n">
-        <v>500</v>
+        <v>665</v>
       </c>
       <c r="J9" t="n">
-        <v>57.249134</v>
+        <v>39.141055</v>
       </c>
       <c r="K9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L9" t="n">
-        <v>45.799307</v>
+        <v>29.355792</v>
       </c>
       <c r="M9" t="n">
-        <v>6200</v>
+        <v>6225</v>
       </c>
       <c r="N9" t="n">
-        <v>520</v>
+        <v>-810</v>
       </c>
       <c r="O9" t="n">
-        <v>760</v>
+        <v>673.75</v>
       </c>
       <c r="P9" t="n">
-        <v>5000</v>
+        <v>6300</v>
       </c>
       <c r="Q9" t="n">
-        <v>150</v>
+        <v>-80</v>
       </c>
       <c r="R9" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S9" t="n">
-        <v>57.749134</v>
+        <v>41.510774</v>
       </c>
       <c r="T9" t="n">
-        <v>5.204866</v>
+        <v>1.686333</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>M3</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>FY3</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.102194</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.994693</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-0.011923</v>
+      </c>
+      <c r="F10" t="n">
+        <v>75</v>
+      </c>
+      <c r="G10" t="n">
+        <v>6300</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-80</v>
+      </c>
+      <c r="I10" t="n">
+        <v>665</v>
+      </c>
+      <c r="J10" t="n">
+        <v>39.141055</v>
+      </c>
+      <c r="K10" t="n">
+        <v>3</v>
+      </c>
+      <c r="L10" t="n">
+        <v>33.269897</v>
+      </c>
+      <c r="M10" t="n">
+        <v>6255</v>
+      </c>
+      <c r="N10" t="n">
+        <v>-518</v>
+      </c>
+      <c r="O10" t="n">
+        <v>670.25</v>
+      </c>
+      <c r="P10" t="n">
+        <v>6320</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>-65</v>
+      </c>
+      <c r="R10" t="n">
+        <v>86</v>
+      </c>
+      <c r="S10" t="n">
+        <v>45.280987</v>
+      </c>
+      <c r="T10" t="n">
+        <v>1.315562</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>FY4</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>-0.914402</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-0.340158</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-0.219457</v>
+      </c>
+      <c r="F11" t="n">
+        <v>120</v>
+      </c>
+      <c r="G11" t="n">
+        <v>6000</v>
+      </c>
+      <c r="H11" t="n">
+        <v>140</v>
+      </c>
+      <c r="I11" t="n">
+        <v>600</v>
+      </c>
+      <c r="J11" t="n">
+        <v>45.567106</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" t="n">
+        <v>29.618619</v>
+      </c>
+      <c r="M11" t="n">
+        <v>7750</v>
+      </c>
+      <c r="N11" t="n">
+        <v>791</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1020</v>
+      </c>
+      <c r="P11" t="n">
+        <v>5980</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>125</v>
+      </c>
+      <c r="R11" t="n">
+        <v>62</v>
+      </c>
+      <c r="S11" t="n">
+        <v>47.544218</v>
+      </c>
+      <c r="T11" t="n">
+        <v>1.950306</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>FY4</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>-0.914402</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-0.340158</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-0.219457</v>
+      </c>
+      <c r="F12" t="n">
+        <v>120</v>
+      </c>
+      <c r="G12" t="n">
+        <v>6000</v>
+      </c>
+      <c r="H12" t="n">
+        <v>140</v>
+      </c>
+      <c r="I12" t="n">
+        <v>600</v>
+      </c>
+      <c r="J12" t="n">
+        <v>45.567106</v>
+      </c>
+      <c r="K12" t="n">
+        <v>2</v>
+      </c>
+      <c r="L12" t="n">
+        <v>34.175329</v>
+      </c>
+      <c r="M12" t="n">
+        <v>7250</v>
+      </c>
+      <c r="N12" t="n">
+        <v>605</v>
+      </c>
+      <c r="O12" t="n">
+        <v>900</v>
+      </c>
+      <c r="P12" t="n">
+        <v>6000</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>140</v>
+      </c>
+      <c r="R12" t="n">
+        <v>74</v>
+      </c>
+      <c r="S12" t="n">
+        <v>51.121232</v>
+      </c>
+      <c r="T12" t="n">
+        <v>1.66809</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>FY4</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>-0.914402</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.340158</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-0.219457</v>
+      </c>
+      <c r="F13" t="n">
+        <v>120</v>
+      </c>
+      <c r="G13" t="n">
+        <v>6000</v>
+      </c>
+      <c r="H13" t="n">
+        <v>140</v>
+      </c>
+      <c r="I13" t="n">
+        <v>600</v>
+      </c>
+      <c r="J13" t="n">
+        <v>45.567106</v>
+      </c>
+      <c r="K13" t="n">
+        <v>3</v>
+      </c>
+      <c r="L13" t="n">
+        <v>38.73204</v>
+      </c>
+      <c r="M13" t="n">
+        <v>6750</v>
+      </c>
+      <c r="N13" t="n">
+        <v>419</v>
+      </c>
+      <c r="O13" t="n">
+        <v>780</v>
+      </c>
+      <c r="P13" t="n">
+        <v>6020</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>155</v>
+      </c>
+      <c r="R13" t="n">
+        <v>86</v>
+      </c>
+      <c r="S13" t="n">
+        <v>54.619829</v>
+      </c>
+      <c r="T13" t="n">
+        <v>1.57893</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>M2</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>FY5</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>-0.96648</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.239519</v>
-      </c>
-      <c r="E10" t="n">
-        <v>-0.092446</v>
-      </c>
-      <c r="F10" t="n">
-        <v>119</v>
-      </c>
-      <c r="G10" t="n">
-        <v>3800</v>
-      </c>
-      <c r="H10" t="n">
-        <v>280</v>
-      </c>
-      <c r="I10" t="n">
-        <v>420</v>
-      </c>
-      <c r="J10" t="n">
-        <v>79.992232</v>
-      </c>
-      <c r="K10" t="n">
+      <c r="C14" t="n">
+        <v>-0.9593469999999999</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.267454</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-0.09012000000000001</v>
+      </c>
+      <c r="F14" t="n">
+        <v>110</v>
+      </c>
+      <c r="G14" t="n">
+        <v>4750</v>
+      </c>
+      <c r="H14" t="n">
+        <v>300</v>
+      </c>
+      <c r="I14" t="n">
+        <v>525</v>
+      </c>
+      <c r="J14" t="n">
+        <v>78.178184</v>
+      </c>
+      <c r="K14" t="n">
         <v>1</v>
       </c>
-      <c r="L10" t="n">
-        <v>63.993785</v>
-      </c>
-      <c r="M10" t="n">
-        <v>5640</v>
-      </c>
-      <c r="N10" t="n">
-        <v>-176</v>
-      </c>
-      <c r="O10" t="n">
-        <v>596</v>
-      </c>
-      <c r="P10" t="n">
-        <v>3800</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>280</v>
-      </c>
-      <c r="R10" t="n">
-        <v>75</v>
-      </c>
-      <c r="S10" t="n">
-        <v>80.492232</v>
-      </c>
-      <c r="T10" t="n">
-        <v>4.305364</v>
+      <c r="L14" t="n">
+        <v>50.81582</v>
+      </c>
+      <c r="M14" t="n">
+        <v>7637.5</v>
+      </c>
+      <c r="N14" t="n">
+        <v>-505</v>
+      </c>
+      <c r="O14" t="n">
+        <v>796.25</v>
+      </c>
+      <c r="P14" t="n">
+        <v>4730</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>285</v>
+      </c>
+      <c r="R14" t="n">
+        <v>62</v>
+      </c>
+      <c r="S14" t="n">
+        <v>79.317865</v>
+      </c>
+      <c r="T14" t="n">
+        <v>1.891709</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>M2</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>FY5</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>-0.9593469999999999</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.267454</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-0.09012000000000001</v>
+      </c>
+      <c r="F15" t="n">
+        <v>110</v>
+      </c>
+      <c r="G15" t="n">
+        <v>4750</v>
+      </c>
+      <c r="H15" t="n">
+        <v>300</v>
+      </c>
+      <c r="I15" t="n">
+        <v>525</v>
+      </c>
+      <c r="J15" t="n">
+        <v>78.178184</v>
+      </c>
+      <c r="K15" t="n">
+        <v>2</v>
+      </c>
+      <c r="L15" t="n">
+        <v>58.633638</v>
+      </c>
+      <c r="M15" t="n">
+        <v>6812.5</v>
+      </c>
+      <c r="N15" t="n">
+        <v>-275</v>
+      </c>
+      <c r="O15" t="n">
+        <v>718.75</v>
+      </c>
+      <c r="P15" t="n">
+        <v>4750</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>300</v>
+      </c>
+      <c r="R15" t="n">
+        <v>74</v>
+      </c>
+      <c r="S15" t="n">
+        <v>79.178184</v>
+      </c>
+      <c r="T15" t="n">
+        <v>1.564661</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>M2</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>FY5</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>-0.9593469999999999</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.267454</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-0.09012000000000001</v>
+      </c>
+      <c r="F16" t="n">
+        <v>110</v>
+      </c>
+      <c r="G16" t="n">
+        <v>4750</v>
+      </c>
+      <c r="H16" t="n">
+        <v>300</v>
+      </c>
+      <c r="I16" t="n">
+        <v>525</v>
+      </c>
+      <c r="J16" t="n">
+        <v>78.178184</v>
+      </c>
+      <c r="K16" t="n">
+        <v>3</v>
+      </c>
+      <c r="L16" t="n">
+        <v>66.451457</v>
+      </c>
+      <c r="M16" t="n">
+        <v>5987.5</v>
+      </c>
+      <c r="N16" t="n">
+        <v>-45</v>
+      </c>
+      <c r="O16" t="n">
+        <v>641.25</v>
+      </c>
+      <c r="P16" t="n">
+        <v>4770</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>315</v>
+      </c>
+      <c r="R16" t="n">
+        <v>86</v>
+      </c>
+      <c r="S16" t="n">
+        <v>79.155981</v>
+      </c>
+      <c r="T16" t="n">
+        <v>1.30243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>